<commit_message>
Manipulação de alguns dados
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21600" windowHeight="8205"/>
+    <workbookView windowWidth="28800" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha de Dados" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>PLANILHA DE DADOS DE COLABORADOR EVENTUAL EXTERNO</t>
   </si>
@@ -79,85 +79,97 @@
     <t>Município:</t>
   </si>
   <si>
+    <t>Coari</t>
+  </si>
+  <si>
+    <t>Ord</t>
+  </si>
+  <si>
+    <t>Nome Completo</t>
+  </si>
+  <si>
+    <t>CPF</t>
+  </si>
+  <si>
+    <t>PIS/PASEP/NIS/NIT</t>
+  </si>
+  <si>
+    <t>RG</t>
+  </si>
+  <si>
+    <t>Órgão Emissor</t>
+  </si>
+  <si>
+    <t>Função</t>
+  </si>
+  <si>
+    <t>Nome do Banco</t>
+  </si>
+  <si>
+    <t>Agência</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Felipe André Souza da Silva</t>
+  </si>
+  <si>
+    <t>2387172-5</t>
+  </si>
+  <si>
+    <t>SSP</t>
+  </si>
+  <si>
+    <t>Aplicador</t>
+  </si>
+  <si>
+    <t>Brasil</t>
+  </si>
+  <si>
+    <t>5786</t>
+  </si>
+  <si>
+    <t>1234-5</t>
+  </si>
+  <si>
+    <t>Adriana Souza da Silva</t>
+  </si>
+  <si>
+    <t>253975-1</t>
+  </si>
+  <si>
+    <t>Apoio</t>
+  </si>
+  <si>
+    <t>Bradesco</t>
+  </si>
+  <si>
+    <t>3726</t>
+  </si>
+  <si>
+    <t>5432-1</t>
+  </si>
+  <si>
+    <t>Municípios</t>
+  </si>
+  <si>
+    <t>Bancos</t>
+  </si>
+  <si>
+    <t>Funções</t>
+  </si>
+  <si>
     <t>Benjamin Constant</t>
   </si>
   <si>
-    <t>Ord</t>
-  </si>
-  <si>
-    <t>Nome Completo</t>
-  </si>
-  <si>
-    <t>CPF</t>
-  </si>
-  <si>
-    <t>PIS/PASEP/NIS/NIT</t>
-  </si>
-  <si>
-    <t>RG</t>
-  </si>
-  <si>
-    <t>Órgão Emissor</t>
-  </si>
-  <si>
-    <t>Função</t>
-  </si>
-  <si>
-    <t>Nome do Banco</t>
-  </si>
-  <si>
-    <t>Agência</t>
-  </si>
-  <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>Felipe André Souza da Silva</t>
-  </si>
-  <si>
-    <t>2387172-5</t>
-  </si>
-  <si>
-    <t>SSP</t>
-  </si>
-  <si>
-    <t>Aplicador</t>
-  </si>
-  <si>
-    <t>Brasil</t>
-  </si>
-  <si>
-    <t>5786</t>
-  </si>
-  <si>
-    <t>1234-5</t>
-  </si>
-  <si>
-    <t>Municípios</t>
-  </si>
-  <si>
-    <t>Bancos</t>
-  </si>
-  <si>
-    <t>Funções</t>
-  </si>
-  <si>
     <t>Agibank</t>
   </si>
   <si>
-    <t>Coari</t>
-  </si>
-  <si>
     <t>Basa</t>
   </si>
   <si>
-    <t>Apoio</t>
-  </si>
-  <si>
     <t>Humaitá</t>
-  </si>
-  <si>
-    <t>Bradesco</t>
   </si>
   <si>
     <t>Porteiro</t>
@@ -195,14 +207,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
-    <numFmt numFmtId="176" formatCode="[$-416]dddd\,\ dd\ &quot;de&quot;\ mmmm\ &quot;de&quot;\ yyyy"/>
-    <numFmt numFmtId="177" formatCode="_-[$R$-416]* #,##0.00_-;\-[$R$-416]* #,##0.00_-;_-[$R$-416]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="000&quot;.&quot;00000&quot;.&quot;00&quot;-&quot;0"/>
-    <numFmt numFmtId="179" formatCode="000&quot;.&quot;000&quot;.&quot;000\-00\ "/>
+    <numFmt numFmtId="176" formatCode="000&quot;.&quot;00000&quot;.&quot;00&quot;-&quot;0"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="[$-416]dddd\,\ dd\ &quot;de&quot;\ mmmm\ &quot;de&quot;\ yyyy"/>
+    <numFmt numFmtId="180" formatCode="_-[$R$-416]* #,##0.00_-;\-[$R$-416]* #,##0.00_-;_-[$R$-416]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="181" formatCode="000&quot;.&quot;000&quot;.&quot;000\-00\ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -244,6 +256,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -251,11 +310,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -267,6 +377,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -275,114 +392,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -403,13 +415,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,169 +511,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -612,6 +624,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -627,11 +663,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -660,17 +702,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -685,175 +721,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -864,16 +876,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -888,27 +900,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -920,7 +932,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1293,13 +1305,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4.28333333333333" style="3" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
@@ -1342,7 +1354,7 @@
       </c>
       <c r="H4" s="20">
         <f ca="1">TODAY()</f>
-        <v>43763</v>
+        <v>43764</v>
       </c>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
@@ -1429,6 +1441,38 @@
       </c>
       <c r="J8" s="24" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="14">
+        <v>2</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="16">
+        <v>47309873220</v>
+      </c>
+      <c r="D9" s="17">
+        <v>20173357886</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1441,10 +1485,10 @@
     <mergeCell ref="H5:J5"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8 H9">
       <formula1>Referências!$C$2:$C$11</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8 G9">
       <formula1>Referências!$E$2:$E$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:J5">
@@ -1479,21 +1523,21 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>20</v>
@@ -1501,68 +1545,68 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="3:3">
       <c r="C8" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="3:3">
       <c r="C9" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="3:3">
       <c r="C10" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="3:3">
       <c r="C11" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reformada formatação de dados e exibição na tela
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -207,14 +207,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
-    <numFmt numFmtId="176" formatCode="000&quot;.&quot;00000&quot;.&quot;00&quot;-&quot;0"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_-[$R$-416]* #,##0.00_-;\-[$R$-416]* #,##0.00_-;_-[$R$-416]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="000&quot;.&quot;00000&quot;.&quot;00&quot;-&quot;0"/>
+    <numFmt numFmtId="178" formatCode="000&quot;.&quot;000&quot;.&quot;000\-00\ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="[$-416]dddd\,\ dd\ &quot;de&quot;\ mmmm\ &quot;de&quot;\ yyyy"/>
-    <numFmt numFmtId="180" formatCode="_-[$R$-416]* #,##0.00_-;\-[$R$-416]* #,##0.00_-;_-[$R$-416]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="181" formatCode="000&quot;.&quot;000&quot;.&quot;000\-00\ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="[$-416]dddd\,\ dd\ &quot;de&quot;\ mmmm\ &quot;de&quot;\ yyyy"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -264,6 +264,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -272,8 +303,90 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,119 +399,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -415,120 +415,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -536,66 +596,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -624,16 +624,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -648,17 +648,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -678,26 +672,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -721,145 +706,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -876,18 +876,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -900,27 +900,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -932,7 +932,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1308,7 +1308,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="H4" s="20">
         <f ca="1">TODAY()</f>
-        <v>43764</v>
+        <v>43770</v>
       </c>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>

</xml_diff>

<commit_message>
Comecei a organizar o projeto e fazer o Javadoc
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="131">
   <si>
     <t>PLANILHA DE DADOS DE COLABORADOR EVENTUAL EXTERNO</t>
   </si>
@@ -73,118 +73,370 @@
     <t>Nome do Local de Aplicação de Prova:</t>
   </si>
   <si>
-    <t>E. E. Cleomenes do Carmo Chaves</t>
+    <t>Escola Estadual Plínio Ramos Ferreira - GM3</t>
   </si>
   <si>
     <t>Município:</t>
   </si>
   <si>
+    <t>Humaitá</t>
+  </si>
+  <si>
+    <t>Ord</t>
+  </si>
+  <si>
+    <t>Nome Completo</t>
+  </si>
+  <si>
+    <t>CPF</t>
+  </si>
+  <si>
+    <t>PIS/PASEP/NIS/NIT</t>
+  </si>
+  <si>
+    <t>RG</t>
+  </si>
+  <si>
+    <t>Órgão Emissor</t>
+  </si>
+  <si>
+    <t>Função</t>
+  </si>
+  <si>
+    <t>Nome do Banco</t>
+  </si>
+  <si>
+    <t>Agência</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>GRACIENE NASCIMENTO DOS SANTOS</t>
+  </si>
+  <si>
+    <t>1557613-2</t>
+  </si>
+  <si>
+    <t>SSP</t>
+  </si>
+  <si>
+    <t>Apoio</t>
+  </si>
+  <si>
+    <t>Bradesco</t>
+  </si>
+  <si>
+    <t>3713-3</t>
+  </si>
+  <si>
+    <t>0623546-8</t>
+  </si>
+  <si>
+    <t>ALDA MARIA UMBELINO ARAÚJO</t>
+  </si>
+  <si>
+    <t>0936675-0</t>
+  </si>
+  <si>
+    <t>Aplicador</t>
+  </si>
+  <si>
+    <t>0624011-9</t>
+  </si>
+  <si>
+    <t>ANA CLAUDIA DA SILVA OLIVEIRA DA CRUZ</t>
+  </si>
+  <si>
+    <t>1504143-3</t>
+  </si>
+  <si>
+    <t>5472-0</t>
+  </si>
+  <si>
+    <t>ANDERSON RAIMUNDO SIQUEI. RELVAS</t>
+  </si>
+  <si>
+    <t>2064656-9</t>
+  </si>
+  <si>
+    <t>0602763-6</t>
+  </si>
+  <si>
+    <t>AUREA MARTINS DE ALMEIDA</t>
+  </si>
+  <si>
+    <t>574695</t>
+  </si>
+  <si>
+    <t>5592-1</t>
+  </si>
+  <si>
+    <t>CLEMILCE MARTINS CORREA MAGALHÃES</t>
+  </si>
+  <si>
+    <t>1141894-0</t>
+  </si>
+  <si>
+    <t>0015088-6</t>
+  </si>
+  <si>
+    <t>DANIELY OLIVEIRA FEITOSA HONDA</t>
+  </si>
+  <si>
+    <t>3251035-7</t>
+  </si>
+  <si>
+    <t>0875-3</t>
+  </si>
+  <si>
+    <t>0572869-0</t>
+  </si>
+  <si>
+    <t>DENIS RAIMUNDO DE OLIVEIRA AQUINO</t>
+  </si>
+  <si>
+    <t>1612213-5</t>
+  </si>
+  <si>
+    <t>5203-5</t>
+  </si>
+  <si>
+    <t>ELIANA LOBATO DOS SANTOS</t>
+  </si>
+  <si>
+    <t>1768840-0</t>
+  </si>
+  <si>
+    <t>2135-0</t>
+  </si>
+  <si>
+    <t>GABRIELE SOUZA BRAZIL</t>
+  </si>
+  <si>
+    <t>1.624.053.606-8</t>
+  </si>
+  <si>
+    <t>2037426-7</t>
+  </si>
+  <si>
+    <t>0015595-0</t>
+  </si>
+  <si>
+    <t>GIZELE CARVALHO LEAL</t>
+  </si>
+  <si>
+    <t>2130230-8</t>
+  </si>
+  <si>
+    <t>0602757-1</t>
+  </si>
+  <si>
+    <t>GOLDWALTER  MAIA BRASIL</t>
+  </si>
+  <si>
+    <t>0869130-4</t>
+  </si>
+  <si>
+    <t>0006432-7</t>
+  </si>
+  <si>
+    <t>GUSTAVO QUEIROZ DA CRUZ</t>
+  </si>
+  <si>
+    <t>1263256</t>
+  </si>
+  <si>
+    <t>Porteiro</t>
+  </si>
+  <si>
+    <t>6336-3</t>
+  </si>
+  <si>
+    <t>7791-7</t>
+  </si>
+  <si>
+    <t>JOAO PAULO FONSECA GUIMARAES_</t>
+  </si>
+  <si>
+    <t>1482556</t>
+  </si>
+  <si>
+    <t>Brasil</t>
+  </si>
+  <si>
+    <t>0926-1</t>
+  </si>
+  <si>
+    <t>27888-2</t>
+  </si>
+  <si>
+    <t>JUCIANE RODRIGUES DE LIMA SOUZA</t>
+  </si>
+  <si>
+    <t>124044804-1</t>
+  </si>
+  <si>
+    <t>10019-6</t>
+  </si>
+  <si>
+    <t>KALINE DOS SANTOS SOUZA</t>
+  </si>
+  <si>
+    <t>2157510-8</t>
+  </si>
+  <si>
+    <t>Caixa</t>
+  </si>
+  <si>
+    <t>4218</t>
+  </si>
+  <si>
+    <t>21617-2</t>
+  </si>
+  <si>
+    <t>MARCIA SILVA DA MOTA</t>
+  </si>
+  <si>
+    <t>1646350-1</t>
+  </si>
+  <si>
+    <t>0013617-4</t>
+  </si>
+  <si>
+    <t>MARIA IVANA TRINDADE DE LIMA</t>
+  </si>
+  <si>
+    <t>1.902.999.498-6</t>
+  </si>
+  <si>
+    <t>1365944-8</t>
+  </si>
+  <si>
+    <t>0015902-6</t>
+  </si>
+  <si>
+    <t>NICÉIA OLIVEIRA LAGO</t>
+  </si>
+  <si>
+    <t>615848</t>
+  </si>
+  <si>
+    <t>Coordenador Local</t>
+  </si>
+  <si>
+    <t>BRASIL</t>
+  </si>
+  <si>
+    <t>14742-7</t>
+  </si>
+  <si>
+    <t>PAULO ROBERTO DE OLIVEIRA LEÃO</t>
+  </si>
+  <si>
+    <t>17989167</t>
+  </si>
+  <si>
+    <t>0008519-7</t>
+  </si>
+  <si>
+    <t>PEDRO AFONSO MORAES DA SILVA</t>
+  </si>
+  <si>
+    <t>19214464</t>
+  </si>
+  <si>
+    <t>16659-6</t>
+  </si>
+  <si>
+    <t>RAIMUNDA DA SILVA MENDONÇA</t>
+  </si>
+  <si>
+    <t>1039892-9</t>
+  </si>
+  <si>
+    <t>0495-2</t>
+  </si>
+  <si>
+    <t>ROSENILDA DE SOUZA TRINDADE</t>
+  </si>
+  <si>
+    <t>765023</t>
+  </si>
+  <si>
+    <t>0003532-7</t>
+  </si>
+  <si>
+    <t>VICENTE ANDRÉ PINTO LEITE SANTOS</t>
+  </si>
+  <si>
+    <t>12756091</t>
+  </si>
+  <si>
+    <t>24025-7</t>
+  </si>
+  <si>
+    <t>ANA MÁRCIA RODRIGUES MOREIRA</t>
+  </si>
+  <si>
+    <t>1823956</t>
+  </si>
+  <si>
+    <t>0603937-5</t>
+  </si>
+  <si>
+    <t>LUCIMAR TICO MIRANDA</t>
+  </si>
+  <si>
+    <t>1769208-3</t>
+  </si>
+  <si>
+    <t>0623990-0</t>
+  </si>
+  <si>
+    <t>MARIA DE FATIMA SILVA DE SOUZA BRASIL</t>
+  </si>
+  <si>
+    <t>0707213-9</t>
+  </si>
+  <si>
+    <t>0012230-0</t>
+  </si>
+  <si>
+    <t>ALDEMIR AGUIAR BARROS</t>
+  </si>
+  <si>
+    <t>17395534</t>
+  </si>
+  <si>
+    <t>2061-3</t>
+  </si>
+  <si>
+    <t>Municípios</t>
+  </si>
+  <si>
+    <t>Bancos</t>
+  </si>
+  <si>
+    <t>Funções</t>
+  </si>
+  <si>
+    <t>Benjamin Constant</t>
+  </si>
+  <si>
+    <t>Agibank</t>
+  </si>
+  <si>
     <t>Coari</t>
   </si>
   <si>
-    <t>Ord</t>
-  </si>
-  <si>
-    <t>Nome Completo</t>
-  </si>
-  <si>
-    <t>CPF</t>
-  </si>
-  <si>
-    <t>PIS/PASEP/NIS/NIT</t>
-  </si>
-  <si>
-    <t>RG</t>
-  </si>
-  <si>
-    <t>Órgão Emissor</t>
-  </si>
-  <si>
-    <t>Função</t>
-  </si>
-  <si>
-    <t>Nome do Banco</t>
-  </si>
-  <si>
-    <t>Agência</t>
-  </si>
-  <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>Felipe André Souza da Silva</t>
-  </si>
-  <si>
-    <t>2387172-5</t>
-  </si>
-  <si>
-    <t>SSP</t>
-  </si>
-  <si>
-    <t>Aplicador</t>
-  </si>
-  <si>
-    <t>Brasil</t>
-  </si>
-  <si>
-    <t>5786</t>
-  </si>
-  <si>
-    <t>1234-5</t>
-  </si>
-  <si>
-    <t>Adriana Souza da Silva</t>
-  </si>
-  <si>
-    <t>253975-1</t>
-  </si>
-  <si>
-    <t>Apoio</t>
-  </si>
-  <si>
-    <t>Bradesco</t>
-  </si>
-  <si>
-    <t>3726</t>
-  </si>
-  <si>
-    <t>5432-1</t>
-  </si>
-  <si>
-    <t>Municípios</t>
-  </si>
-  <si>
-    <t>Bancos</t>
-  </si>
-  <si>
-    <t>Funções</t>
-  </si>
-  <si>
-    <t>Benjamin Constant</t>
-  </si>
-  <si>
-    <t>Agibank</t>
-  </si>
-  <si>
     <t>Basa</t>
   </si>
   <si>
-    <t>Humaitá</t>
-  </si>
-  <si>
-    <t>Porteiro</t>
-  </si>
-  <si>
     <t>Itacoatiara</t>
   </si>
   <si>
-    <t>Coordenador Local</t>
-  </si>
-  <si>
     <t>Parintins</t>
-  </si>
-  <si>
-    <t>Caixa</t>
   </si>
   <si>
     <t>Inter</t>
@@ -207,14 +459,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
-    <numFmt numFmtId="176" formatCode="_-[$R$-416]* #,##0.00_-;\-[$R$-416]* #,##0.00_-;_-[$R$-416]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="000&quot;.&quot;00000&quot;.&quot;00&quot;-&quot;0"/>
+    <numFmt numFmtId="176" formatCode="000&quot;.&quot;00000&quot;.&quot;00&quot;-&quot;0"/>
+    <numFmt numFmtId="177" formatCode="[$-416]dddd\,\ dd\ &quot;de&quot;\ mmmm\ &quot;de&quot;\ yyyy"/>
     <numFmt numFmtId="178" formatCode="000&quot;.&quot;000&quot;.&quot;000\-00\ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="[$-416]dddd\,\ dd\ &quot;de&quot;\ mmmm\ &quot;de&quot;\ yyyy"/>
+    <numFmt numFmtId="180" formatCode="_-[$R$-416]* #,##0.00_-;\-[$R$-416]* #,##0.00_-;_-[$R$-416]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="181" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -264,14 +516,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -288,6 +532,81 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -296,7 +615,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -312,29 +638,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -347,58 +651,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -415,25 +667,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -445,157 +829,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -624,17 +876,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -644,15 +890,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -668,6 +905,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -696,17 +948,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -721,145 +962,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -879,13 +1131,13 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -903,7 +1155,7 @@
     <xf numFmtId="178" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -913,14 +1165,14 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -932,7 +1184,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1305,10 +1557,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1354,7 +1606,7 @@
       </c>
       <c r="H4" s="20">
         <f ca="1">TODAY()</f>
-        <v>43770</v>
+        <v>43777</v>
       </c>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
@@ -1364,12 +1616,12 @@
         <v>3</v>
       </c>
       <c r="B5" s="10"/>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
       <c r="G5" s="21" t="s">
         <v>5</v>
       </c>
@@ -1419,10 +1671,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="16">
-        <v>930816269</v>
+        <v>61809349249</v>
       </c>
       <c r="D8" s="17">
-        <v>20173357886</v>
+        <v>12879553654</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>18</v>
@@ -1451,10 +1703,10 @@
         <v>24</v>
       </c>
       <c r="C9" s="16">
-        <v>47309873220</v>
+        <v>345439022</v>
       </c>
       <c r="D9" s="17">
-        <v>20173357886</v>
+        <v>160268310</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>25</v>
@@ -1466,16 +1718,851 @@
         <v>26</v>
       </c>
       <c r="H9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="23" t="s">
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="14">
+        <v>3</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="24" t="s">
+      <c r="C10" s="16">
+        <v>66954789291</v>
+      </c>
+      <c r="D10" s="17">
+        <v>12645038656</v>
+      </c>
+      <c r="E10" s="23" t="s">
         <v>29</v>
       </c>
+      <c r="F10" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="14">
+        <v>4</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="16">
+        <v>574978267</v>
+      </c>
+      <c r="D11" s="17">
+        <v>19048270289</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="14">
+        <v>5</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="16">
+        <v>59344032220</v>
+      </c>
+      <c r="D12" s="17">
+        <v>12581110653</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="14">
+        <v>6</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="16">
+        <v>34545166253</v>
+      </c>
+      <c r="D13" s="17">
+        <v>17059918319</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="14">
+        <v>7</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="16">
+        <v>391483277</v>
+      </c>
+      <c r="D14" s="17">
+        <v>12871900657</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="14">
+        <v>8</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="16">
+        <v>51868075249</v>
+      </c>
+      <c r="D15" s="17">
+        <v>19025887697</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="14">
+        <v>9</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="16">
+        <v>51199173215</v>
+      </c>
+      <c r="D16" s="17">
+        <v>16153911707</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="14">
+        <v>10</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="16">
+        <v>99121700249</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="14">
+        <v>11</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="16">
+        <v>93271026220</v>
+      </c>
+      <c r="D18" s="17">
+        <v>12806992658</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="14">
+        <v>12</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="16">
+        <v>31512690287</v>
+      </c>
+      <c r="D19" s="17">
+        <v>12326733861</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="14">
+        <v>13</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="16">
+        <v>2597966208</v>
+      </c>
+      <c r="D20" s="17">
+        <v>21036205241</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="14">
+        <v>14</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="16">
+        <v>87376997253</v>
+      </c>
+      <c r="D21" s="17">
+        <v>20615809418</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="14">
+        <v>15</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="16">
+        <v>58427600291</v>
+      </c>
+      <c r="D22" s="17">
+        <v>19030419884</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="14">
+        <v>16</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="16">
+        <v>1642986224</v>
+      </c>
+      <c r="D23" s="17">
+        <v>21007646405</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="J23" s="24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="14">
+        <v>17</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="16">
+        <v>995706962</v>
+      </c>
+      <c r="D24" s="17">
+        <v>1641586918</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="14">
+        <v>18</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="16">
+        <v>62824015268</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="14">
+        <v>19</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="16">
+        <v>77142160268</v>
+      </c>
+      <c r="D26" s="17">
+        <v>16618234027</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="J26" s="24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="14">
+        <v>20</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="16">
+        <v>77765699253</v>
+      </c>
+      <c r="D27" s="17">
+        <v>20632290557</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="14">
+        <v>21</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="16">
+        <v>1657182266</v>
+      </c>
+      <c r="D28" s="17">
+        <v>11997110703</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="14">
+        <v>22</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="16">
+        <v>34359087268</v>
+      </c>
+      <c r="D29" s="17">
+        <v>12420849630</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" s="24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="14">
+        <v>23</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="16">
+        <v>86239821268</v>
+      </c>
+      <c r="D30" s="17">
+        <v>16630831633</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" s="24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="14">
+        <v>24</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="16">
+        <v>59472790291</v>
+      </c>
+      <c r="D31" s="17">
+        <v>17059918343</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="I31" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="J31" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="14">
+        <v>25</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="16">
+        <v>80099165287</v>
+      </c>
+      <c r="D32" s="17">
+        <v>16123281357</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="14">
+        <v>26</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="16">
+        <v>76076598204</v>
+      </c>
+      <c r="D33" s="17">
+        <v>16441268230</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J33" s="24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="14">
+        <v>27</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="16">
+        <v>23090782200</v>
+      </c>
+      <c r="D34" s="17">
+        <v>12420977876</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J34" s="24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="14">
+        <v>28</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="16">
+        <v>21978794215</v>
+      </c>
+      <c r="D35" s="17">
+        <v>12183355133</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J35" s="24" t="s">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="B33:J35">
+    <sortCondition ref="B33:B35"/>
+  </sortState>
   <mergeCells count="6">
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A4:E4"/>
@@ -1485,10 +2572,10 @@
     <mergeCell ref="H5:J5"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8 H9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H35">
       <formula1>Referências!$C$2:$C$11</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8 G9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G20 G26 G8:G12 G13:G15 G16:G19 G21:G25 G27:G35">
       <formula1>Referências!$E$2:$E$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:J5">
@@ -1523,90 +2610,90 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>121</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>122</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>123</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>124</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>125</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="3:3">
       <c r="C8" s="2" t="s">
-        <v>43</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="3:3">
       <c r="C9" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="3:3">
       <c r="C10" s="2" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="3:3">
       <c r="C11" s="2" t="s">
-        <v>46</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>